<commit_message>
updated some of the paper
</commit_message>
<xml_diff>
--- a/reports/charts.xlsx
+++ b/reports/charts.xlsx
@@ -1,25 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <workbookPr hidePivotFieldList="1" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dukef\projects\data_structures\Sorting-Algorithms-DataStructures\reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6BC3FB7-8427-4C61-A7DA-94E502B7DF7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{506978F1-0309-459D-BD90-3681A6F54925}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30" yWindow="0" windowWidth="38445" windowHeight="20910" xr2:uid="{86A1B264-82BA-4240-B491-5D92586D73D2}"/>
+    <workbookView xWindow="19125" yWindow="0" windowWidth="19290" windowHeight="20910" xr2:uid="{86A1B264-82BA-4240-B491-5D92586D73D2}"/>
   </bookViews>
   <sheets>
     <sheet name="booksdata" sheetId="2" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">booksdata!$A$52:$C$112</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="61" r:id="rId2"/>
-    <pivotCache cacheId="67" r:id="rId3"/>
-    <pivotCache cacheId="71" r:id="rId4"/>
+    <pivotCache cacheId="0" r:id="rId2"/>
+    <pivotCache cacheId="1" r:id="rId3"/>
+    <pivotCache cacheId="2" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -175,13 +178,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1117,6 +1119,664 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Ints</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> up to 100</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>booksdata!$B$52</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Insertionsort Ints(ms)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>booksdata!$A$53:$A$103</c:f>
+              <c:strCache>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>AlmostInOrder_10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>AlmostInOrder_10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>AlmostInOrder_10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>AlmostInOrder_100</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>AlmostInOrder_100</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>AlmostInOrder_100</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>InOrder_10</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>InOrder_10</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>InOrder_10</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>InOrder_100</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>InOrder_100</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>InOrder_100</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>RandomOrder_10</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>RandomOrder_10</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>RandomOrder_10</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>RandomOrder_100</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>RandomOrder_100</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>RandomOrder_100</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>ReverseOrder_10</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>ReverseOrder_10</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>ReverseOrder_10</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>ReverseOrder_100</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>ReverseOrder_100</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>ReverseOrder_100</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>booksdata!$B$53:$B$103</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-29BD-4FAB-8F70-2DC6944F9333}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>booksdata!$C$52</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Mergesort Ints(ms)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>booksdata!$A$53:$A$103</c:f>
+              <c:strCache>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>AlmostInOrder_10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>AlmostInOrder_10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>AlmostInOrder_10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>AlmostInOrder_100</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>AlmostInOrder_100</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>AlmostInOrder_100</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>InOrder_10</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>InOrder_10</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>InOrder_10</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>InOrder_100</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>InOrder_100</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>InOrder_100</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>RandomOrder_10</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>RandomOrder_10</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>RandomOrder_10</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>RandomOrder_100</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>RandomOrder_100</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>RandomOrder_100</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>ReverseOrder_10</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>ReverseOrder_10</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>ReverseOrder_10</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>ReverseOrder_100</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>ReverseOrder_100</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>ReverseOrder_100</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>booksdata!$C$53:$C$103</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-29BD-4FAB-8F70-2DC6944F9333}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="182"/>
+        <c:axId val="423068624"/>
+        <c:axId val="423069104"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="423068624"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="423069104"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="423069104"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="423068624"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
@@ -5447,7 +6107,7 @@
             <c:strRef>
               <c:f>booksdata!$A$53:$A$112</c:f>
               <c:strCache>
-                <c:ptCount val="60"/>
+                <c:ptCount val="24"/>
                 <c:pt idx="0">
                   <c:v>AlmostInOrder_10</c:v>
                 </c:pt>
@@ -5467,166 +6127,58 @@
                   <c:v>AlmostInOrder_100</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>AlmostInOrder_1000</c:v>
+                  <c:v>InOrder_10</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>AlmostInOrder_1000</c:v>
+                  <c:v>InOrder_10</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>AlmostInOrder_1000</c:v>
+                  <c:v>InOrder_10</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>AlmostInOrder_10000</c:v>
+                  <c:v>InOrder_100</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>AlmostInOrder_10000</c:v>
+                  <c:v>InOrder_100</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>AlmostInOrder_10000</c:v>
+                  <c:v>InOrder_100</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>AlmostInOrder_100000</c:v>
+                  <c:v>RandomOrder_10</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>AlmostInOrder_100000</c:v>
+                  <c:v>RandomOrder_10</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>AlmostInOrder_100000</c:v>
+                  <c:v>RandomOrder_10</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>InOrder_10</c:v>
+                  <c:v>RandomOrder_100</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>InOrder_10</c:v>
+                  <c:v>RandomOrder_100</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>InOrder_10</c:v>
+                  <c:v>RandomOrder_100</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>InOrder_100</c:v>
+                  <c:v>ReverseOrder_10</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>InOrder_100</c:v>
+                  <c:v>ReverseOrder_10</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>InOrder_100</c:v>
+                  <c:v>ReverseOrder_10</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>InOrder_1000</c:v>
+                  <c:v>ReverseOrder_100</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>InOrder_1000</c:v>
+                  <c:v>ReverseOrder_100</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>InOrder_1000</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>InOrder_10000</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>InOrder_10000</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>InOrder_10000</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>InOrder_100000</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>InOrder_100000</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>InOrder_100000</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>RandomOrder_10</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>RandomOrder_10</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>RandomOrder_10</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>RandomOrder_100</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>RandomOrder_100</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>RandomOrder_100</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>RandomOrder_1000</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>RandomOrder_1000</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>RandomOrder_1000</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>RandomOrder_10000</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>RandomOrder_10000</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>RandomOrder_10000</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>RandomOrder_100000</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>RandomOrder_100000</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>RandomOrder_100000</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>ReverseOrder_10</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>ReverseOrder_10</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>ReverseOrder_10</c:v>
-                </c:pt>
-                <c:pt idx="48">
                   <c:v>ReverseOrder_100</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>ReverseOrder_100</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>ReverseOrder_100</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>ReverseOrder_1000</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>ReverseOrder_1000</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>ReverseOrder_1000</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>ReverseOrder_10000</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>ReverseOrder_10000</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>ReverseOrder_10000</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>ReverseOrder_100000</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>ReverseOrder_100000</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>ReverseOrder_100000</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -5636,7 +6188,7 @@
               <c:f>booksdata!$B$53:$B$112</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="60"/>
+                <c:ptCount val="24"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -5665,22 +6217,22 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>33</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>33</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>33</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3262</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3272</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3279</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>0</c:v>
@@ -5708,114 +6260,6 @@
                 </c:pt>
                 <c:pt idx="23">
                   <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>137</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>138</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>137</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>13680</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>13730</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>13655</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>272</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>275</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>273</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>27424</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>27414</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>27464</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5854,7 +6298,7 @@
             <c:strRef>
               <c:f>booksdata!$A$53:$A$112</c:f>
               <c:strCache>
-                <c:ptCount val="60"/>
+                <c:ptCount val="24"/>
                 <c:pt idx="0">
                   <c:v>AlmostInOrder_10</c:v>
                 </c:pt>
@@ -5874,166 +6318,58 @@
                   <c:v>AlmostInOrder_100</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>AlmostInOrder_1000</c:v>
+                  <c:v>InOrder_10</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>AlmostInOrder_1000</c:v>
+                  <c:v>InOrder_10</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>AlmostInOrder_1000</c:v>
+                  <c:v>InOrder_10</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>AlmostInOrder_10000</c:v>
+                  <c:v>InOrder_100</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>AlmostInOrder_10000</c:v>
+                  <c:v>InOrder_100</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>AlmostInOrder_10000</c:v>
+                  <c:v>InOrder_100</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>AlmostInOrder_100000</c:v>
+                  <c:v>RandomOrder_10</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>AlmostInOrder_100000</c:v>
+                  <c:v>RandomOrder_10</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>AlmostInOrder_100000</c:v>
+                  <c:v>RandomOrder_10</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>InOrder_10</c:v>
+                  <c:v>RandomOrder_100</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>InOrder_10</c:v>
+                  <c:v>RandomOrder_100</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>InOrder_10</c:v>
+                  <c:v>RandomOrder_100</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>InOrder_100</c:v>
+                  <c:v>ReverseOrder_10</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>InOrder_100</c:v>
+                  <c:v>ReverseOrder_10</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>InOrder_100</c:v>
+                  <c:v>ReverseOrder_10</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>InOrder_1000</c:v>
+                  <c:v>ReverseOrder_100</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>InOrder_1000</c:v>
+                  <c:v>ReverseOrder_100</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>InOrder_1000</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>InOrder_10000</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>InOrder_10000</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>InOrder_10000</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>InOrder_100000</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>InOrder_100000</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>InOrder_100000</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>RandomOrder_10</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>RandomOrder_10</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>RandomOrder_10</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>RandomOrder_100</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>RandomOrder_100</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>RandomOrder_100</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>RandomOrder_1000</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>RandomOrder_1000</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>RandomOrder_1000</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>RandomOrder_10000</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>RandomOrder_10000</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>RandomOrder_10000</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>RandomOrder_100000</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>RandomOrder_100000</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>RandomOrder_100000</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>ReverseOrder_10</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>ReverseOrder_10</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>ReverseOrder_10</c:v>
-                </c:pt>
-                <c:pt idx="48">
                   <c:v>ReverseOrder_100</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>ReverseOrder_100</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>ReverseOrder_100</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>ReverseOrder_1000</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>ReverseOrder_1000</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>ReverseOrder_1000</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>ReverseOrder_10000</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>ReverseOrder_10000</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>ReverseOrder_10000</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>ReverseOrder_100000</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>ReverseOrder_100000</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>ReverseOrder_100000</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -6043,7 +6379,7 @@
               <c:f>booksdata!$C$53:$C$112</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="60"/>
+                <c:ptCount val="24"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -6069,160 +6405,52 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="22">
                   <c:v>16</c:v>
                 </c:pt>
-                <c:pt idx="10">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="23">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>24</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6534,7 +6762,7 @@
             <c:strRef>
               <c:f>booksdata!$A$53:$A$112</c:f>
               <c:strCache>
-                <c:ptCount val="60"/>
+                <c:ptCount val="24"/>
                 <c:pt idx="0">
                   <c:v>AlmostInOrder_10</c:v>
                 </c:pt>
@@ -6554,166 +6782,58 @@
                   <c:v>AlmostInOrder_100</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>AlmostInOrder_1000</c:v>
+                  <c:v>InOrder_10</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>AlmostInOrder_1000</c:v>
+                  <c:v>InOrder_10</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>AlmostInOrder_1000</c:v>
+                  <c:v>InOrder_10</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>AlmostInOrder_10000</c:v>
+                  <c:v>InOrder_100</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>AlmostInOrder_10000</c:v>
+                  <c:v>InOrder_100</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>AlmostInOrder_10000</c:v>
+                  <c:v>InOrder_100</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>AlmostInOrder_100000</c:v>
+                  <c:v>RandomOrder_10</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>AlmostInOrder_100000</c:v>
+                  <c:v>RandomOrder_10</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>AlmostInOrder_100000</c:v>
+                  <c:v>RandomOrder_10</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>InOrder_10</c:v>
+                  <c:v>RandomOrder_100</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>InOrder_10</c:v>
+                  <c:v>RandomOrder_100</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>InOrder_10</c:v>
+                  <c:v>RandomOrder_100</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>InOrder_100</c:v>
+                  <c:v>ReverseOrder_10</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>InOrder_100</c:v>
+                  <c:v>ReverseOrder_10</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>InOrder_100</c:v>
+                  <c:v>ReverseOrder_10</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>InOrder_1000</c:v>
+                  <c:v>ReverseOrder_100</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>InOrder_1000</c:v>
+                  <c:v>ReverseOrder_100</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>InOrder_1000</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>InOrder_10000</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>InOrder_10000</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>InOrder_10000</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>InOrder_100000</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>InOrder_100000</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>InOrder_100000</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>RandomOrder_10</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>RandomOrder_10</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>RandomOrder_10</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>RandomOrder_100</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>RandomOrder_100</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>RandomOrder_100</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>RandomOrder_1000</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>RandomOrder_1000</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>RandomOrder_1000</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>RandomOrder_10000</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>RandomOrder_10000</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>RandomOrder_10000</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>RandomOrder_100000</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>RandomOrder_100000</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>RandomOrder_100000</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>ReverseOrder_10</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>ReverseOrder_10</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>ReverseOrder_10</c:v>
-                </c:pt>
-                <c:pt idx="48">
                   <c:v>ReverseOrder_100</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>ReverseOrder_100</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>ReverseOrder_100</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>ReverseOrder_1000</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>ReverseOrder_1000</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>ReverseOrder_1000</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>ReverseOrder_10000</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>ReverseOrder_10000</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>ReverseOrder_10000</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>ReverseOrder_100000</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>ReverseOrder_100000</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>ReverseOrder_100000</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -6723,7 +6843,7 @@
               <c:f>booksdata!$B$53:$B$112</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="60"/>
+                <c:ptCount val="24"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -6752,22 +6872,22 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>33</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>33</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>33</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3262</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3272</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3279</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>0</c:v>
@@ -6795,114 +6915,6 @@
                 </c:pt>
                 <c:pt idx="23">
                   <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>137</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>138</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>137</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>13680</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>13730</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>13655</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>272</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>275</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>273</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>27424</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>27414</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>27464</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6944,7 +6956,7 @@
             <c:strRef>
               <c:f>booksdata!$A$53:$A$112</c:f>
               <c:strCache>
-                <c:ptCount val="60"/>
+                <c:ptCount val="24"/>
                 <c:pt idx="0">
                   <c:v>AlmostInOrder_10</c:v>
                 </c:pt>
@@ -6964,166 +6976,58 @@
                   <c:v>AlmostInOrder_100</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>AlmostInOrder_1000</c:v>
+                  <c:v>InOrder_10</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>AlmostInOrder_1000</c:v>
+                  <c:v>InOrder_10</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>AlmostInOrder_1000</c:v>
+                  <c:v>InOrder_10</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>AlmostInOrder_10000</c:v>
+                  <c:v>InOrder_100</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>AlmostInOrder_10000</c:v>
+                  <c:v>InOrder_100</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>AlmostInOrder_10000</c:v>
+                  <c:v>InOrder_100</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>AlmostInOrder_100000</c:v>
+                  <c:v>RandomOrder_10</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>AlmostInOrder_100000</c:v>
+                  <c:v>RandomOrder_10</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>AlmostInOrder_100000</c:v>
+                  <c:v>RandomOrder_10</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>InOrder_10</c:v>
+                  <c:v>RandomOrder_100</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>InOrder_10</c:v>
+                  <c:v>RandomOrder_100</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>InOrder_10</c:v>
+                  <c:v>RandomOrder_100</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>InOrder_100</c:v>
+                  <c:v>ReverseOrder_10</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>InOrder_100</c:v>
+                  <c:v>ReverseOrder_10</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>InOrder_100</c:v>
+                  <c:v>ReverseOrder_10</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>InOrder_1000</c:v>
+                  <c:v>ReverseOrder_100</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>InOrder_1000</c:v>
+                  <c:v>ReverseOrder_100</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>InOrder_1000</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>InOrder_10000</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>InOrder_10000</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>InOrder_10000</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>InOrder_100000</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>InOrder_100000</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>InOrder_100000</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>RandomOrder_10</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>RandomOrder_10</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>RandomOrder_10</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>RandomOrder_100</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>RandomOrder_100</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>RandomOrder_100</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>RandomOrder_1000</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>RandomOrder_1000</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>RandomOrder_1000</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>RandomOrder_10000</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>RandomOrder_10000</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>RandomOrder_10000</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>RandomOrder_100000</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>RandomOrder_100000</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>RandomOrder_100000</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>ReverseOrder_10</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>ReverseOrder_10</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>ReverseOrder_10</c:v>
-                </c:pt>
-                <c:pt idx="48">
                   <c:v>ReverseOrder_100</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>ReverseOrder_100</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>ReverseOrder_100</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>ReverseOrder_1000</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>ReverseOrder_1000</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>ReverseOrder_1000</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>ReverseOrder_10000</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>ReverseOrder_10000</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>ReverseOrder_10000</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>ReverseOrder_100000</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>ReverseOrder_100000</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>ReverseOrder_100000</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -7133,7 +7037,7 @@
               <c:f>booksdata!$C$53:$C$112</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="60"/>
+                <c:ptCount val="24"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -7159,160 +7063,52 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="22">
                   <c:v>16</c:v>
                 </c:pt>
-                <c:pt idx="10">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="23">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>24</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7721,8 +7517,8 @@
     <c:plotArea>
       <c:layout/>
       <c:barChart>
-        <c:barDir val="bar"/>
-        <c:grouping val="stacked"/>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -8067,7 +7863,6 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="55"/>
-        <c:overlap val="100"/>
         <c:axId val="1229523119"/>
         <c:axId val="1229526479"/>
       </c:barChart>
@@ -8077,7 +7872,7 @@
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
-        <c:axPos val="l"/>
+        <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -8128,7 +7923,7 @@
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
-        <c:axPos val="b"/>
+        <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -10159,6 +9954,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors10.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -10995,6 +10830,511 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style10.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
   <cs:axisTitle>
@@ -15265,15 +15605,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>218514</xdr:colOff>
-      <xdr:row>78</xdr:row>
-      <xdr:rowOff>174812</xdr:rowOff>
+      <xdr:colOff>218513</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>554690</xdr:colOff>
-      <xdr:row>93</xdr:row>
-      <xdr:rowOff>60512</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>1129391</xdr:colOff>
+      <xdr:row>127</xdr:row>
+      <xdr:rowOff>176892</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -15365,6 +15705,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId9"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>285749</xdr:colOff>
+      <xdr:row>133</xdr:row>
+      <xdr:rowOff>179614</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>204106</xdr:colOff>
+      <xdr:row>148</xdr:row>
+      <xdr:rowOff>65314</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="11" name="Chart 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1445758C-3D26-FC14-465C-94C197C4E464}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId10"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -16398,7 +16774,190 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{67F914CF-8E2E-43A4-B0BC-A6093910B312}" name="PivotTable49" cacheId="71" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{0A5C3B18-095D-4C4A-B43F-F98BF83881AD}" name="PivotTable46" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="20">
+  <location ref="D115:F136" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="3">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="21">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item x="13"/>
+        <item x="14"/>
+        <item x="15"/>
+        <item x="16"/>
+        <item x="17"/>
+        <item x="18"/>
+        <item x="19"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="21">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="11"/>
+    </i>
+    <i>
+      <x v="12"/>
+    </i>
+    <i>
+      <x v="13"/>
+    </i>
+    <i>
+      <x v="14"/>
+    </i>
+    <i>
+      <x v="15"/>
+    </i>
+    <i>
+      <x v="16"/>
+    </i>
+    <i>
+      <x v="17"/>
+    </i>
+    <i>
+      <x v="18"/>
+    </i>
+    <i>
+      <x v="19"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Average of Insertionsort Ints(ms)" fld="1" subtotal="average" baseField="0" baseItem="0"/>
+    <dataField name="Average of Mergesort Ints(ms)" fld="2" subtotal="average" baseField="0" baseItem="0"/>
+  </dataFields>
+  <chartFormats count="6">
+    <chartFormat chart="0" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="1" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="16" format="2" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="16" format="3" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="17" format="4" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="17" format="5" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{67F914CF-8E2E-43A4-B0BC-A6093910B312}" name="PivotTable49" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="6">
   <location ref="Q13:S30" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField axis="axisRow" showAll="0">
@@ -16528,8 +17087,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B50AA515-4A95-46FD-9761-C40A169BCC81}" name="PivotTable48" cacheId="67" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="10">
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B50AA515-4A95-46FD-9761-C40A169BCC81}" name="PivotTable48" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="10">
   <location ref="Q58:U75" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField axis="axisRow" showAll="0">
@@ -16670,153 +17229,6 @@
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
             <x v="3"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{0A5C3B18-095D-4C4A-B43F-F98BF83881AD}" name="PivotTable46" cacheId="61" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
-  <location ref="D115:F136" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="3">
-    <pivotField axis="axisRow" showAll="0">
-      <items count="21">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="8"/>
-        <item x="9"/>
-        <item x="10"/>
-        <item x="11"/>
-        <item x="12"/>
-        <item x="13"/>
-        <item x="14"/>
-        <item x="15"/>
-        <item x="16"/>
-        <item x="17"/>
-        <item x="18"/>
-        <item x="19"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="0"/>
-  </rowFields>
-  <rowItems count="21">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="8"/>
-    </i>
-    <i>
-      <x v="9"/>
-    </i>
-    <i>
-      <x v="10"/>
-    </i>
-    <i>
-      <x v="11"/>
-    </i>
-    <i>
-      <x v="12"/>
-    </i>
-    <i>
-      <x v="13"/>
-    </i>
-    <i>
-      <x v="14"/>
-    </i>
-    <i>
-      <x v="15"/>
-    </i>
-    <i>
-      <x v="16"/>
-    </i>
-    <i>
-      <x v="17"/>
-    </i>
-    <i>
-      <x v="18"/>
-    </i>
-    <i>
-      <x v="19"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="-2"/>
-  </colFields>
-  <colItems count="2">
-    <i>
-      <x/>
-    </i>
-    <i i="1">
-      <x v="1"/>
-    </i>
-  </colItems>
-  <dataFields count="2">
-    <dataField name="Average of Insertionsort Ints(ms)" fld="1" subtotal="average" baseField="0" baseItem="0"/>
-    <dataField name="Average of Mergesort Ints(ms)" fld="2" subtotal="average" baseField="0" baseItem="0"/>
-  </dataFields>
-  <chartFormats count="2">
-    <chartFormat chart="0" format="0" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="1" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="1"/>
           </reference>
         </references>
       </pivotArea>
@@ -17151,10 +17563,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EF18658-BA29-4DD8-84E8-A25C0F958686}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:U136"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="U22" sqref="U22"/>
+    <sheetView tabSelected="1" topLeftCell="P28" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="T43" sqref="T43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17421,10 +17834,10 @@
       <c r="Q14" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="R14" s="3">
-        <v>0</v>
-      </c>
-      <c r="S14" s="3">
+      <c r="R14">
+        <v>0</v>
+      </c>
+      <c r="S14">
         <v>0</v>
       </c>
     </row>
@@ -17447,10 +17860,10 @@
       <c r="Q15" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="R15" s="3">
-        <v>0</v>
-      </c>
-      <c r="S15" s="3">
+      <c r="R15">
+        <v>0</v>
+      </c>
+      <c r="S15">
         <v>4.333333333333333</v>
       </c>
     </row>
@@ -17473,10 +17886,10 @@
       <c r="Q16" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="R16" s="3">
+      <c r="R16">
         <v>3</v>
       </c>
-      <c r="S16" s="3">
+      <c r="S16">
         <v>3</v>
       </c>
     </row>
@@ -17499,10 +17912,10 @@
       <c r="Q17" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="R17" s="3">
+      <c r="R17">
         <v>307.33333333333331</v>
       </c>
-      <c r="S17" s="3">
+      <c r="S17">
         <v>5.333333333333333</v>
       </c>
     </row>
@@ -17525,10 +17938,10 @@
       <c r="Q18" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="R18" s="3">
-        <v>0</v>
-      </c>
-      <c r="S18" s="3">
+      <c r="R18">
+        <v>0</v>
+      </c>
+      <c r="S18">
         <v>0</v>
       </c>
     </row>
@@ -17551,10 +17964,10 @@
       <c r="Q19" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="R19" s="3">
-        <v>0</v>
-      </c>
-      <c r="S19" s="3">
+      <c r="R19">
+        <v>0</v>
+      </c>
+      <c r="S19">
         <v>3</v>
       </c>
     </row>
@@ -17577,10 +17990,10 @@
       <c r="Q20" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="R20" s="3">
-        <v>0</v>
-      </c>
-      <c r="S20" s="3">
+      <c r="R20">
+        <v>0</v>
+      </c>
+      <c r="S20">
         <v>4.333333333333333</v>
       </c>
     </row>
@@ -17603,10 +18016,10 @@
       <c r="Q21" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="R21" s="3">
+      <c r="R21">
         <v>1</v>
       </c>
-      <c r="S21" s="3">
+      <c r="S21">
         <v>2.3333333333333335</v>
       </c>
     </row>
@@ -17629,10 +18042,10 @@
       <c r="Q22" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="R22" s="3">
-        <v>0</v>
-      </c>
-      <c r="S22" s="3">
+      <c r="R22">
+        <v>0</v>
+      </c>
+      <c r="S22">
         <v>0</v>
       </c>
     </row>
@@ -17655,10 +18068,10 @@
       <c r="Q23" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="R23" s="3">
-        <v>0</v>
-      </c>
-      <c r="S23" s="3">
+      <c r="R23">
+        <v>0</v>
+      </c>
+      <c r="S23">
         <v>5</v>
       </c>
     </row>
@@ -17681,10 +18094,10 @@
       <c r="Q24" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="R24" s="3">
+      <c r="R24">
         <v>11</v>
       </c>
-      <c r="S24" s="3">
+      <c r="S24">
         <v>3</v>
       </c>
     </row>
@@ -17707,10 +18120,10 @@
       <c r="Q25" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="R25" s="3">
+      <c r="R25">
         <v>1307.6666666666667</v>
       </c>
-      <c r="S25" s="3">
+      <c r="S25">
         <v>4.666666666666667</v>
       </c>
     </row>
@@ -17733,10 +18146,10 @@
       <c r="Q26" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="R26" s="3">
-        <v>0</v>
-      </c>
-      <c r="S26" s="3">
+      <c r="R26">
+        <v>0</v>
+      </c>
+      <c r="S26">
         <v>0</v>
       </c>
     </row>
@@ -17759,10 +18172,10 @@
       <c r="Q27" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="R27" s="3">
-        <v>0</v>
-      </c>
-      <c r="S27" s="3">
+      <c r="R27">
+        <v>0</v>
+      </c>
+      <c r="S27">
         <v>2.3333333333333335</v>
       </c>
     </row>
@@ -17785,10 +18198,10 @@
       <c r="Q28" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="R28" s="3">
+      <c r="R28">
         <v>22.666666666666668</v>
       </c>
-      <c r="S28" s="3">
+      <c r="S28">
         <v>5</v>
       </c>
     </row>
@@ -17811,10 +18224,10 @@
       <c r="Q29" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="R29" s="3">
+      <c r="R29">
         <v>2450.6666666666665</v>
       </c>
-      <c r="S29" s="3">
+      <c r="S29">
         <v>3</v>
       </c>
     </row>
@@ -17837,10 +18250,10 @@
       <c r="Q30" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="R30" s="3">
+      <c r="R30">
         <v>256.45833333333331</v>
       </c>
-      <c r="S30" s="3">
+      <c r="S30">
         <v>2.8333333333333335</v>
       </c>
     </row>
@@ -18264,7 +18677,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="59" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>13</v>
       </c>
@@ -18277,20 +18690,20 @@
       <c r="Q59" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="R59" s="3">
-        <v>0</v>
-      </c>
-      <c r="S59" s="3">
-        <v>0</v>
-      </c>
-      <c r="T59" s="3">
-        <v>0</v>
-      </c>
-      <c r="U59" s="3">
+      <c r="R59">
+        <v>0</v>
+      </c>
+      <c r="S59">
+        <v>0</v>
+      </c>
+      <c r="T59">
+        <v>0</v>
+      </c>
+      <c r="U59">
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>13</v>
       </c>
@@ -18303,20 +18716,20 @@
       <c r="Q60" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="R60" s="3">
-        <v>0</v>
-      </c>
-      <c r="S60" s="3">
+      <c r="R60">
+        <v>0</v>
+      </c>
+      <c r="S60">
         <v>4.333333333333333</v>
       </c>
-      <c r="T60" s="3">
-        <v>0</v>
-      </c>
-      <c r="U60" s="3">
+      <c r="T60">
+        <v>0</v>
+      </c>
+      <c r="U60">
         <v>8.3333333333333339</v>
       </c>
     </row>
-    <row r="61" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>13</v>
       </c>
@@ -18329,20 +18742,20 @@
       <c r="Q61" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="R61" s="3">
+      <c r="R61">
         <v>3</v>
       </c>
-      <c r="S61" s="3">
+      <c r="S61">
         <v>3</v>
       </c>
-      <c r="T61" s="3">
-        <v>0</v>
-      </c>
-      <c r="U61" s="3">
+      <c r="T61">
+        <v>0</v>
+      </c>
+      <c r="U61">
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="62" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>12</v>
       </c>
@@ -18355,20 +18768,20 @@
       <c r="Q62" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="R62" s="3">
+      <c r="R62">
         <v>307.33333333333331</v>
       </c>
-      <c r="S62" s="3">
+      <c r="S62">
         <v>5.333333333333333</v>
       </c>
-      <c r="T62" s="3">
+      <c r="T62">
         <v>33</v>
       </c>
-      <c r="U62" s="3">
+      <c r="U62">
         <v>5.333333333333333</v>
       </c>
     </row>
-    <row r="63" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>12</v>
       </c>
@@ -18381,20 +18794,20 @@
       <c r="Q63" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="R63" s="3">
-        <v>0</v>
-      </c>
-      <c r="S63" s="3">
-        <v>0</v>
-      </c>
-      <c r="T63" s="3">
-        <v>0</v>
-      </c>
-      <c r="U63" s="3">
+      <c r="R63">
+        <v>0</v>
+      </c>
+      <c r="S63">
+        <v>0</v>
+      </c>
+      <c r="T63">
+        <v>0</v>
+      </c>
+      <c r="U63">
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>12</v>
       </c>
@@ -18407,20 +18820,20 @@
       <c r="Q64" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="R64" s="3">
-        <v>0</v>
-      </c>
-      <c r="S64" s="3">
+      <c r="R64">
+        <v>0</v>
+      </c>
+      <c r="S64">
         <v>3</v>
       </c>
-      <c r="T64" s="3">
-        <v>0</v>
-      </c>
-      <c r="U64" s="3">
+      <c r="T64">
+        <v>0</v>
+      </c>
+      <c r="U64">
         <v>11</v>
       </c>
     </row>
-    <row r="65" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>22</v>
       </c>
@@ -18433,20 +18846,20 @@
       <c r="Q65" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="R65" s="3">
-        <v>0</v>
-      </c>
-      <c r="S65" s="3">
+      <c r="R65">
+        <v>0</v>
+      </c>
+      <c r="S65">
         <v>4.333333333333333</v>
       </c>
-      <c r="T65" s="3">
-        <v>0</v>
-      </c>
-      <c r="U65" s="3">
+      <c r="T65">
+        <v>0</v>
+      </c>
+      <c r="U65">
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="66" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>22</v>
       </c>
@@ -18459,20 +18872,20 @@
       <c r="Q66" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="R66" s="3">
+      <c r="R66">
         <v>1</v>
       </c>
-      <c r="S66" s="3">
+      <c r="S66">
         <v>2.3333333333333335</v>
       </c>
-      <c r="T66" s="3">
-        <v>0</v>
-      </c>
-      <c r="U66" s="3">
+      <c r="T66">
+        <v>0</v>
+      </c>
+      <c r="U66">
         <v>7.333333333333333</v>
       </c>
     </row>
-    <row r="67" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>22</v>
       </c>
@@ -18485,16 +18898,16 @@
       <c r="Q67" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="R67" s="3">
-        <v>0</v>
-      </c>
-      <c r="S67" s="3">
-        <v>0</v>
-      </c>
-      <c r="T67" s="3">
-        <v>0</v>
-      </c>
-      <c r="U67" s="3">
+      <c r="R67">
+        <v>0</v>
+      </c>
+      <c r="S67">
+        <v>0</v>
+      </c>
+      <c r="T67">
+        <v>0</v>
+      </c>
+      <c r="U67">
         <v>0</v>
       </c>
     </row>
@@ -18511,16 +18924,16 @@
       <c r="Q68" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="R68" s="3">
-        <v>0</v>
-      </c>
-      <c r="S68" s="3">
+      <c r="R68">
+        <v>0</v>
+      </c>
+      <c r="S68">
         <v>5</v>
       </c>
-      <c r="T68" s="3">
-        <v>0</v>
-      </c>
-      <c r="U68" s="3">
+      <c r="T68">
+        <v>0</v>
+      </c>
+      <c r="U68">
         <v>9</v>
       </c>
     </row>
@@ -18537,16 +18950,16 @@
       <c r="Q69" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="R69" s="3">
+      <c r="R69">
         <v>11</v>
       </c>
-      <c r="S69" s="3">
+      <c r="S69">
         <v>3</v>
       </c>
-      <c r="T69" s="3">
+      <c r="T69">
         <v>1</v>
       </c>
-      <c r="U69" s="3">
+      <c r="U69">
         <v>0.33333333333333331</v>
       </c>
     </row>
@@ -18563,16 +18976,16 @@
       <c r="Q70" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="R70" s="3">
+      <c r="R70">
         <v>1307.6666666666667</v>
       </c>
-      <c r="S70" s="3">
+      <c r="S70">
         <v>4.666666666666667</v>
       </c>
-      <c r="T70" s="3">
+      <c r="T70">
         <v>137.33333333333334</v>
       </c>
-      <c r="U70" s="3">
+      <c r="U70">
         <v>6</v>
       </c>
     </row>
@@ -18589,16 +19002,16 @@
       <c r="Q71" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="R71" s="3">
-        <v>0</v>
-      </c>
-      <c r="S71" s="3">
-        <v>0</v>
-      </c>
-      <c r="T71" s="3">
-        <v>0</v>
-      </c>
-      <c r="U71" s="3">
+      <c r="R71">
+        <v>0</v>
+      </c>
+      <c r="S71">
+        <v>0</v>
+      </c>
+      <c r="T71">
+        <v>0</v>
+      </c>
+      <c r="U71">
         <v>0</v>
       </c>
     </row>
@@ -18615,16 +19028,16 @@
       <c r="Q72" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="R72" s="3">
-        <v>0</v>
-      </c>
-      <c r="S72" s="3">
+      <c r="R72">
+        <v>0</v>
+      </c>
+      <c r="S72">
         <v>2.3333333333333335</v>
       </c>
-      <c r="T72" s="3">
-        <v>0</v>
-      </c>
-      <c r="U72" s="3">
+      <c r="T72">
+        <v>0</v>
+      </c>
+      <c r="U72">
         <v>5.666666666666667</v>
       </c>
     </row>
@@ -18641,20 +19054,20 @@
       <c r="Q73" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="R73" s="3">
+      <c r="R73">
         <v>22.666666666666668</v>
       </c>
-      <c r="S73" s="3">
+      <c r="S73">
         <v>5</v>
       </c>
-      <c r="T73" s="3">
+      <c r="T73">
         <v>2</v>
       </c>
-      <c r="U73" s="3">
+      <c r="U73">
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="74" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>9</v>
       </c>
@@ -18667,20 +19080,20 @@
       <c r="Q74" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="R74" s="3">
+      <c r="R74">
         <v>2450.6666666666665</v>
       </c>
-      <c r="S74" s="3">
+      <c r="S74">
         <v>3</v>
       </c>
-      <c r="T74" s="3">
+      <c r="T74">
         <v>273.33333333333331</v>
       </c>
-      <c r="U74" s="3">
+      <c r="U74">
         <v>8.3333333333333339</v>
       </c>
     </row>
-    <row r="75" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>9</v>
       </c>
@@ -18693,20 +19106,20 @@
       <c r="Q75" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="R75" s="3">
+      <c r="R75">
         <v>256.45833333333331</v>
       </c>
-      <c r="S75" s="3">
+      <c r="S75">
         <v>2.8333333333333335</v>
       </c>
-      <c r="T75" s="3">
+      <c r="T75">
         <v>27.916666666666668</v>
       </c>
-      <c r="U75" s="3">
+      <c r="U75">
         <v>3.9375</v>
       </c>
     </row>
-    <row r="76" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>9</v>
       </c>
@@ -18717,7 +19130,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="77" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>8</v>
       </c>
@@ -18728,7 +19141,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="78" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>8</v>
       </c>
@@ -18739,7 +19152,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>8</v>
       </c>
@@ -18750,7 +19163,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>23</v>
       </c>
@@ -18761,7 +19174,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>23</v>
       </c>
@@ -18772,7 +19185,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>23</v>
       </c>
@@ -18849,7 +19262,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>5</v>
       </c>
@@ -18860,7 +19273,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>5</v>
       </c>
@@ -18871,7 +19284,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>5</v>
       </c>
@@ -18882,7 +19295,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>4</v>
       </c>
@@ -18893,7 +19306,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>4</v>
       </c>
@@ -18904,7 +19317,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>4</v>
       </c>
@@ -18915,7 +19328,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>24</v>
       </c>
@@ -18926,7 +19339,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>24</v>
       </c>
@@ -18937,7 +19350,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>24</v>
       </c>
@@ -19014,7 +19427,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>1</v>
       </c>
@@ -19025,7 +19438,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>1</v>
       </c>
@@ -19036,7 +19449,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>1</v>
       </c>
@@ -19047,7 +19460,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>0</v>
       </c>
@@ -19058,7 +19471,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>0</v>
       </c>
@@ -19069,7 +19482,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>0</v>
       </c>
@@ -19080,7 +19493,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>25</v>
       </c>
@@ -19091,7 +19504,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>25</v>
       </c>
@@ -19102,7 +19515,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>25</v>
       </c>
@@ -19128,10 +19541,10 @@
       <c r="D116" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E116" s="3">
-        <v>0</v>
-      </c>
-      <c r="F116" s="3">
+      <c r="E116">
+        <v>0</v>
+      </c>
+      <c r="F116">
         <v>0</v>
       </c>
     </row>
@@ -19139,10 +19552,10 @@
       <c r="D117" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E117" s="3">
-        <v>0</v>
-      </c>
-      <c r="F117" s="3">
+      <c r="E117">
+        <v>0</v>
+      </c>
+      <c r="F117">
         <v>8.3333333333333339</v>
       </c>
     </row>
@@ -19150,10 +19563,10 @@
       <c r="D118" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E118" s="3">
-        <v>0</v>
-      </c>
-      <c r="F118" s="3">
+      <c r="E118">
+        <v>0</v>
+      </c>
+      <c r="F118">
         <v>0.33333333333333331</v>
       </c>
     </row>
@@ -19161,10 +19574,10 @@
       <c r="D119" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E119" s="3">
+      <c r="E119">
         <v>33</v>
       </c>
-      <c r="F119" s="3">
+      <c r="F119">
         <v>5.333333333333333</v>
       </c>
     </row>
@@ -19172,10 +19585,10 @@
       <c r="D120" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E120" s="3">
+      <c r="E120">
         <v>3271</v>
       </c>
-      <c r="F120" s="3">
+      <c r="F120">
         <v>9</v>
       </c>
     </row>
@@ -19183,10 +19596,10 @@
       <c r="D121" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E121" s="3">
-        <v>0</v>
-      </c>
-      <c r="F121" s="3">
+      <c r="E121">
+        <v>0</v>
+      </c>
+      <c r="F121">
         <v>0</v>
       </c>
     </row>
@@ -19194,10 +19607,10 @@
       <c r="D122" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E122" s="3">
-        <v>0</v>
-      </c>
-      <c r="F122" s="3">
+      <c r="E122">
+        <v>0</v>
+      </c>
+      <c r="F122">
         <v>11</v>
       </c>
     </row>
@@ -19205,10 +19618,10 @@
       <c r="D123" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E123" s="3">
-        <v>0</v>
-      </c>
-      <c r="F123" s="3">
+      <c r="E123">
+        <v>0</v>
+      </c>
+      <c r="F123">
         <v>0.66666666666666663</v>
       </c>
     </row>
@@ -19216,10 +19629,10 @@
       <c r="D124" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E124" s="3">
-        <v>0</v>
-      </c>
-      <c r="F124" s="3">
+      <c r="E124">
+        <v>0</v>
+      </c>
+      <c r="F124">
         <v>7.333333333333333</v>
       </c>
     </row>
@@ -19227,10 +19640,10 @@
       <c r="D125" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E125" s="3">
-        <v>0</v>
-      </c>
-      <c r="F125" s="3">
+      <c r="E125">
+        <v>0</v>
+      </c>
+      <c r="F125">
         <v>6</v>
       </c>
     </row>
@@ -19238,10 +19651,10 @@
       <c r="D126" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E126" s="3">
-        <v>0</v>
-      </c>
-      <c r="F126" s="3">
+      <c r="E126">
+        <v>0</v>
+      </c>
+      <c r="F126">
         <v>0</v>
       </c>
     </row>
@@ -19249,10 +19662,10 @@
       <c r="D127" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E127" s="3">
-        <v>0</v>
-      </c>
-      <c r="F127" s="3">
+      <c r="E127">
+        <v>0</v>
+      </c>
+      <c r="F127">
         <v>9</v>
       </c>
     </row>
@@ -19260,10 +19673,10 @@
       <c r="D128" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E128" s="3">
+      <c r="E128">
         <v>1</v>
       </c>
-      <c r="F128" s="3">
+      <c r="F128">
         <v>0.33333333333333331</v>
       </c>
     </row>
@@ -19271,10 +19684,10 @@
       <c r="D129" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E129" s="3">
+      <c r="E129">
         <v>137.33333333333334</v>
       </c>
-      <c r="F129" s="3">
+      <c r="F129">
         <v>6</v>
       </c>
     </row>
@@ -19282,10 +19695,10 @@
       <c r="D130" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E130" s="3">
+      <c r="E130">
         <v>13688.333333333334</v>
       </c>
-      <c r="F130" s="3">
+      <c r="F130">
         <v>8</v>
       </c>
     </row>
@@ -19293,10 +19706,10 @@
       <c r="D131" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E131" s="3">
-        <v>0</v>
-      </c>
-      <c r="F131" s="3">
+      <c r="E131">
+        <v>0</v>
+      </c>
+      <c r="F131">
         <v>0</v>
       </c>
     </row>
@@ -19304,10 +19717,10 @@
       <c r="D132" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E132" s="3">
-        <v>0</v>
-      </c>
-      <c r="F132" s="3">
+      <c r="E132">
+        <v>0</v>
+      </c>
+      <c r="F132">
         <v>5.666666666666667</v>
       </c>
     </row>
@@ -19315,10 +19728,10 @@
       <c r="D133" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E133" s="3">
+      <c r="E133">
         <v>2</v>
       </c>
-      <c r="F133" s="3">
+      <c r="F133">
         <v>0.66666666666666663</v>
       </c>
     </row>
@@ -19326,10 +19739,10 @@
       <c r="D134" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="E134" s="3">
+      <c r="E134">
         <v>273.33333333333331</v>
       </c>
-      <c r="F134" s="3">
+      <c r="F134">
         <v>8.3333333333333339</v>
       </c>
     </row>
@@ -19337,10 +19750,10 @@
       <c r="D135" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E135" s="3">
+      <c r="E135">
         <v>27434</v>
       </c>
-      <c r="F135" s="3">
+      <c r="F135">
         <v>8.3333333333333339</v>
       </c>
     </row>
@@ -19348,14 +19761,28 @@
       <c r="D136" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E136" s="3">
+      <c r="E136">
         <v>2242</v>
       </c>
-      <c r="F136" s="3">
+      <c r="F136">
         <v>4.7166666666666668</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A52:C112" xr:uid="{7EF18658-BA29-4DD8-84E8-A25C0F958686}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="AlmostInOrder_10"/>
+        <filter val="AlmostInOrder_100"/>
+        <filter val="InOrder_10"/>
+        <filter val="InOrder_100"/>
+        <filter val="RandomOrder_10"/>
+        <filter val="RandomOrder_100"/>
+        <filter val="ReverseOrder_10"/>
+        <filter val="ReverseOrder_100"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId4"/>
 </worksheet>

</xml_diff>